<commit_message>
Added consecutive nights function
</commit_message>
<xml_diff>
--- a/RESULTS/Week_12_Year_2024/(0) סידור מוכן.xlsx
+++ b/RESULTS/Week_12_Year_2024/(0) סידור מוכן.xlsx
@@ -710,32 +710,32 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>אמור</t>
+          <t>רוני</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>אמור</t>
+          <t>רוני</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>morning.noon.night</t>
+          <t>morning.noon</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
+          <t>morning.night</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>morning.noon</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
-        </is>
-      </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>morning.noon</t>
+          <t>morning.night</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -745,12 +745,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>morning.noon.night</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
+          <t>night</t>
         </is>
       </c>
       <c r="T2" t="n">
@@ -782,32 +777,32 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
+          <t>morning.noon</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>morning.noon.night</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>noon</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>morning.noon</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
           <t>noon.night</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>morning</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>noon.night</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -827,49 +822,49 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
+          <t>אוראל</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>רוני</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>אמור</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>זיו</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>אמור</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>אמור</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
           <t>יניב</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>זיו</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>אמור</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>אמור</t>
         </is>
       </c>
-      <c r="F4" s="6" t="inlineStr">
-        <is>
-          <t>זיו</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>זיו</t>
-        </is>
-      </c>
-      <c r="H4" s="7" t="inlineStr">
-        <is>
-          <t>יניב</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>עמית</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>עמית</t>
-        </is>
-      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>morning.noon.night</t>
@@ -877,17 +872,17 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>morning.noon.night</t>
+          <t>morning.noon</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>noon.night</t>
+          <t>morning.noon.night</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>morning.noon.night</t>
+          <t>morning.noon</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -897,12 +892,12 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>morning</t>
+          <t>morning.noon.night</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>night</t>
+          <t>morning.noon.night</t>
         </is>
       </c>
       <c r="T4" t="n">
@@ -917,77 +912,82 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
           <t>זיו</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>יניב</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>אור</t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>אור</t>
-        </is>
-      </c>
-      <c r="F5" s="6" t="inlineStr">
-        <is>
-          <t>אמור</t>
-        </is>
-      </c>
       <c r="G5" s="7" t="inlineStr">
         <is>
-          <t>אמור</t>
+          <t>זיו</t>
         </is>
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>אמור</t>
+          <t>זיו</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>רוני</t>
+          <t>עמית</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>רוני</t>
+          <t>עמית</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
+          <t>morning.noon.night</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>morning.noon.night</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>noon.night</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>morning.noon.night</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>morning.noon.night</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>morning</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
           <t>night</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>morning.night</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>noon.night</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>morning</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>morning.noon.night</t>
         </is>
       </c>
       <c r="T5" t="n">
@@ -1002,37 +1002,37 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
+          <t>עמית</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>זיו</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>עמית</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>יניב</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>רוני</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
           <t>אמור</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>עמית</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>זיו</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>יניב</t>
-        </is>
-      </c>
-      <c r="F6" s="9" t="inlineStr">
-        <is>
-          <t>אור</t>
-        </is>
-      </c>
-      <c r="G6" s="7" t="inlineStr">
-        <is>
-          <t>אור</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>אוראל</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1150,7 +1150,7 @@
       <c r="G8" s="5" t="n"/>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>זיו</t>
+          <t>אור</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1215,12 +1215,12 @@
       <c r="F9" s="6" t="n"/>
       <c r="G9" s="7" t="inlineStr">
         <is>
+          <t>יניב</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr">
+        <is>
           <t>אוראל</t>
-        </is>
-      </c>
-      <c r="H9" s="7" t="inlineStr">
-        <is>
-          <t>רוני</t>
         </is>
       </c>
       <c r="J9" s="24" t="inlineStr">
@@ -1237,24 +1237,24 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
+          <t>אמור</t>
+        </is>
+      </c>
+      <c r="C10" s="25" t="inlineStr">
+        <is>
+          <t>תגבור</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
           <t>אוראל</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>רוני</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr">
-        <is>
-          <t>רוני</t>
-        </is>
-      </c>
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>עמית</t>
-        </is>
-      </c>
       <c r="F10" s="13" t="inlineStr">
         <is>
           <t>אוראל</t>
@@ -1270,6 +1270,7 @@
           <t>תגבור</t>
         </is>
       </c>
+      <c r="J10" s="24" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="22" t="inlineStr">

</xml_diff>